<commit_message>
Update Bug sheet Greenlam WMS  15 April.xlsx
</commit_message>
<xml_diff>
--- a/Bug sheet Greenlam WMS  15 April.xlsx
+++ b/Bug sheet Greenlam WMS  15 April.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Summery" sheetId="1" r:id="rId1"/>
@@ -3025,8 +3025,8 @@
   </sheetPr>
   <dimension ref="A1:O994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3215,10 +3215,10 @@
         <v>36</v>
       </c>
       <c r="F10" s="57">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="G10" s="16">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -3242,10 +3242,10 @@
         <v>36</v>
       </c>
       <c r="F11" s="57">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G11" s="16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3269,10 +3269,10 @@
         <v>36</v>
       </c>
       <c r="F12" s="57">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="G12" s="16">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -3297,11 +3297,11 @@
       </c>
       <c r="F13" s="57">
         <f>SUM(F10:F12)</f>
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="G13" s="12">
         <f>SUM(G10:G12)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -20005,7 +20005,7 @@
   </sheetPr>
   <dimension ref="A1:AC994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S94" sqref="S94"/>
     </sheetView>
   </sheetViews>

</xml_diff>